<commit_message>
able to read description from matlab file and convert it into
</commit_message>
<xml_diff>
--- a/spectrometer/scan.xlsx
+++ b/spectrometer/scan.xlsx
@@ -684,28 +684,75 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Reflection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> peak vs RH at 20C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.3422104526553947E-2"/>
-          <c:y val="1.4552128036196006E-2"/>
-          <c:w val="0.92633563280135356"/>
-          <c:h val="0.90939357545086985"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>sample_1</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -728,61 +775,70 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>scan!$E$2:$E$18</c:f>
+              <c:f>scan!$E$4:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>619.45111083984295</c:v>
+                  <c:v>446.20687866210898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>446.20687866210898</c:v>
+                  <c:v>428.32711791992102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>446.20687866210898</c:v>
+                  <c:v>459.74645996093699</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>428.32711791992102</c:v>
+                  <c:v>435.91342163085898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>459.74645996093699</c:v>
+                  <c:v>434.82974243164</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>435.91342163085898</c:v>
+                  <c:v>456.497467041015</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>434.82974243164</c:v>
+                  <c:v>465.16079711914</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>456.497467041015</c:v>
+                  <c:v>463.53662109375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>465.16079711914</c:v>
+                  <c:v>436.45526123046801</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>463.53662109375</c:v>
+                  <c:v>427.24325561523398</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>436.45526123046801</c:v>
+                  <c:v>427.24325561523398</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>427.24325561523398</c:v>
+                  <c:v>481.93899536132801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>427.24325561523398</c:v>
+                  <c:v>433.20416259765602</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>481.93899536132801</c:v>
+                  <c:v>433.20416259765602</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>433.20416259765602</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>433.20416259765602</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>474.36294555664</c:v>
                 </c:pt>
               </c:numCache>
@@ -790,56 +846,53 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scan!$D$2:$D$18</c:f>
+              <c:f>scan!$D$4:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>50.19</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.19</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>22.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>65.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>75</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83</c:v>
+                  <c:v>17.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="16">
                   <c:v>80.319999999999993</c:v>
                 </c:pt>
               </c:numCache>
@@ -849,134 +902,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EDD0-41C6-B980-30A3575A4790}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>sample_2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>scan!$E$19:$E$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>455.41439819335898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>427.24325561523398</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>426.15933227539</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>427.24325561523398</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>457.038970947265</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>428.869049072265</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>433.20416259765602</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>435.91342163085898</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>454.33126831054602</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>453.78970336914</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>459.74645996093699</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>464.078033447265</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>433.74603271484301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>scan!$D$19:$D$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.72</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70.47</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27.92</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>67.62</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>67.62</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>72.17</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>76.36</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>30.57</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EDD0-41C6-B980-30A3575A4790}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1000,20 +925,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Peak wavelength</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38287326987352388"/>
+              <c:y val="0.89026258792558566"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1036,7 +1010,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1059,6 +1033,8 @@
         <c:axId val="330196624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1076,6 +1052,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> humidity at 20C(%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1098,7 +1134,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1149,7 +1185,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1722,16 +1758,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>421481</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>30954</xdr:rowOff>
+      <xdr:rowOff>183354</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2058,13 +2094,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2098,7 +2134,7 @@
         <v>0.101292525427575</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2118,7 +2154,7 @@
         <v>0.54411237726653705</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2138,7 +2174,7 @@
         <v>0.54554576076829298</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>0.55315945520244603</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2178,7 +2214,7 @@
         <v>0.52794629251602898</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2198,7 +2234,7 @@
         <v>0.541994056100639</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2218,7 +2254,7 @@
         <v>0.53865979381443296</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2238,7 +2274,7 @@
         <v>0.51793640728326795</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2258,7 +2294,7 @@
         <v>0.51093724837618704</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2278,7 +2314,7 @@
         <v>0.51056728178050104</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2298,7 +2334,7 @@
         <v>0.52991850518695205</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2318,7 +2354,7 @@
         <v>0.52338992764524594</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2338,7 +2374,7 @@
         <v>0.53511474078849897</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2358,7 +2394,7 @@
         <v>0.48517229864380101</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2378,7 +2414,7 @@
         <v>0.52664082797393397</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2398,7 +2434,7 @@
         <v>0.52940925933813099</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2418,7 +2454,7 @@
         <v>0.49666112139459601</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2435,7 +2471,7 @@
         <v>0.52354527938342899</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2455,7 +2491,7 @@
         <v>0.535687847744585</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2475,7 +2511,7 @@
         <v>0.53499325401692599</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2495,7 +2531,7 @@
         <v>0.53258351839912099</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2515,7 +2551,7 @@
         <v>0.52720028758013204</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2535,7 +2571,7 @@
         <v>0.54307925847555005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2555,7 +2591,7 @@
         <v>0.54231440862046898</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2575,7 +2611,7 @@
         <v>0.54246223995440201</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2595,7 +2631,7 @@
         <v>0.54887676458173695</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2615,7 +2651,7 @@
         <v>0.55023802768056995</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2635,7 +2671,7 @@
         <v>0.51959403122394399</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2655,7 +2691,7 @@
         <v>0.52968904948854101</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>